<commit_message>
Created vaxCEA_CISNETvaxCompare.m to produce outputs for CISNET vax compare analysis
</commit_message>
<xml_diff>
--- a/Config/Weights_costs.xlsx
+++ b/Config/Weights_costs.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Costs" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -105,8 +105,11 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Not currently used.</t>
+      <t>Not currently used. Hard-coded into vaxCEA analysis.</t>
     </r>
+  </si>
+  <si>
+    <t>Later redefined/ hard-coded into vaxCEA analysis.</t>
   </si>
   <si>
     <r>
@@ -119,7 +122,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Not currently used.</t>
+      <t>Not currently used. Hard-coded into vaxCEA analysis.</t>
     </r>
   </si>
 </sst>
@@ -222,7 +225,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -250,9 +253,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -537,7 +542,7 @@
   <dimension ref="A1:AB39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -547,7 +552,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="2"/>
@@ -632,7 +637,7 @@
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="16">
         <v>117.03849292812023</v>
       </c>
       <c r="C4" s="5"/>
@@ -650,7 +655,7 @@
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="16">
         <v>56.017155398551346</v>
       </c>
       <c r="C5" s="5"/>
@@ -668,7 +673,7 @@
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="16">
         <v>37.666707940405217</v>
       </c>
       <c r="C6" s="5"/>
@@ -686,7 +691,7 @@
       <c r="A7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="16">
         <v>38</v>
       </c>
       <c r="C7" s="5"/>
@@ -704,7 +709,7 @@
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="17">
+      <c r="B8" s="16">
         <f>37.6667079404052+B10</f>
         <v>297.6032853811551</v>
       </c>
@@ -979,7 +984,7 @@
     </row>
     <row r="25" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A25" s="14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1013,7 +1018,7 @@
       <c r="A26" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="17">
+      <c r="B26" s="16">
         <v>27</v>
       </c>
       <c r="C26" s="5" t="s">
@@ -1081,50 +1086,70 @@
       <c r="L31" s="5"/>
     </row>
     <row r="32" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
+      <c r="A32" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+      <c r="Y32" s="1"/>
+      <c r="Z32" s="1"/>
+      <c r="AA32" s="1"/>
+      <c r="AB32" s="1"/>
     </row>
     <row r="33" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="1"/>
-      <c r="R33" s="1"/>
-      <c r="S33" s="1"/>
-      <c r="T33" s="1"/>
-      <c r="U33" s="1"/>
-      <c r="V33" s="1"/>
-      <c r="W33" s="1"/>
-      <c r="X33" s="1"/>
-      <c r="Y33" s="1"/>
-      <c r="Z33" s="1"/>
-      <c r="AA33" s="1"/>
-      <c r="AB33" s="1"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
+      <c r="O33" s="19"/>
+      <c r="P33" s="19"/>
+      <c r="Q33" s="19"/>
+      <c r="R33" s="19"/>
+      <c r="S33" s="19"/>
+      <c r="T33" s="19"/>
+      <c r="U33" s="19"/>
+      <c r="V33" s="19"/>
+      <c r="W33" s="19"/>
+      <c r="X33" s="19"/>
+      <c r="Y33" s="19"/>
+      <c r="Z33" s="19"/>
+      <c r="AA33" s="19"/>
+      <c r="AB33" s="19"/>
     </row>
     <row r="34" spans="1:28" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
@@ -1224,5 +1249,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>